<commit_message>
手続中一览、手続詳細 Signed-off-by: LiuYiYang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_ホワイトボート_問い合わせ履歴.xlsx
+++ b/test_物件管理/test_ホワイトボート_問い合わせ履歴.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="574">
   <si>
     <t>URL:</t>
   </si>
@@ -1215,15 +1215,7 @@
     <t>看板</t>
   </si>
   <si>
-    <t>看板</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>知人紹介</t>
-  </si>
-  <si>
-    <t>知人紹介</t>
-    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>id_created_user</t>
@@ -1586,13 +1578,6 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>SHOT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>問い合わせ一覧表示</t>
-  </si>
-  <si>
     <t>3</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
@@ -2066,6 +2051,10 @@
   <si>
     <t>002-005-005</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3050,7 +3039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -3061,7 +3050,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="113" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="102" customFormat="1" ht="14.25">
@@ -3069,7 +3058,7 @@
         <v>181</v>
       </c>
       <c r="B2" s="113" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="102" customFormat="1" ht="14.25">
@@ -3077,7 +3066,7 @@
         <v>181</v>
       </c>
       <c r="B3" s="116" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="102" customFormat="1" ht="14.25">
@@ -3085,7 +3074,7 @@
         <v>181</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="102" customFormat="1" ht="14.25">
@@ -3093,7 +3082,7 @@
         <v>181</v>
       </c>
       <c r="B5" s="113" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25">
@@ -3101,7 +3090,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25">
@@ -3109,7 +3098,7 @@
         <v>181</v>
       </c>
       <c r="B7" s="116" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25">
@@ -3125,7 +3114,7 @@
         <v>181</v>
       </c>
       <c r="B9" s="116" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25">
@@ -3133,7 +3122,7 @@
         <v>181</v>
       </c>
       <c r="B10" s="116" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25">
@@ -3141,7 +3130,7 @@
         <v>181</v>
       </c>
       <c r="B11" s="116" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25">
@@ -3149,7 +3138,7 @@
         <v>181</v>
       </c>
       <c r="B12" s="116" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25">
@@ -3157,7 +3146,7 @@
         <v>181</v>
       </c>
       <c r="B13" s="116" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.25">
@@ -3181,7 +3170,7 @@
         <v>181</v>
       </c>
       <c r="B16" s="116" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25">
@@ -3189,7 +3178,7 @@
         <v>181</v>
       </c>
       <c r="B17" s="116" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25">
@@ -3205,7 +3194,7 @@
         <v>181</v>
       </c>
       <c r="B19" s="116" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25">
@@ -3213,7 +3202,7 @@
         <v>181</v>
       </c>
       <c r="B20" s="116" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25">
@@ -3221,7 +3210,7 @@
         <v>181</v>
       </c>
       <c r="B21" s="116" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25">
@@ -3229,7 +3218,7 @@
         <v>181</v>
       </c>
       <c r="B22" s="116" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25">
@@ -3237,7 +3226,7 @@
         <v>181</v>
       </c>
       <c r="B23" s="116" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25">
@@ -3245,7 +3234,7 @@
         <v>181</v>
       </c>
       <c r="B24" s="116" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25">
@@ -3253,7 +3242,7 @@
         <v>181</v>
       </c>
       <c r="B25" s="116" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25">
@@ -3261,7 +3250,7 @@
         <v>181</v>
       </c>
       <c r="B26" s="116" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25">
@@ -3269,7 +3258,7 @@
         <v>181</v>
       </c>
       <c r="B27" s="116" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25">
@@ -3277,7 +3266,7 @@
         <v>181</v>
       </c>
       <c r="B28" s="116" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25">
@@ -3285,7 +3274,7 @@
         <v>181</v>
       </c>
       <c r="B29" s="116" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25">
@@ -3293,7 +3282,7 @@
         <v>181</v>
       </c>
       <c r="B30" s="116" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25">
@@ -3301,7 +3290,7 @@
         <v>181</v>
       </c>
       <c r="B31" s="116" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25">
@@ -3309,7 +3298,7 @@
         <v>181</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="33" spans="1:75" ht="14.25">
@@ -3317,7 +3306,7 @@
         <v>181</v>
       </c>
       <c r="B33" s="116" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="34" spans="1:75" ht="14.25">
@@ -3325,7 +3314,7 @@
         <v>181</v>
       </c>
       <c r="B34" s="116" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="35" spans="1:75" ht="14.25">
@@ -3333,7 +3322,7 @@
         <v>181</v>
       </c>
       <c r="B35" s="116" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="36" spans="1:75" ht="14.25">
@@ -3341,7 +3330,7 @@
         <v>181</v>
       </c>
       <c r="B36" s="116" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="37" spans="1:75" ht="14.25">
@@ -3349,7 +3338,7 @@
         <v>181</v>
       </c>
       <c r="B37" s="116" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="38" spans="1:75" ht="14.25">
@@ -3357,7 +3346,7 @@
         <v>181</v>
       </c>
       <c r="B38" s="116" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="39" spans="1:75" ht="14.25">
@@ -3527,7 +3516,7 @@
         <v>181</v>
       </c>
       <c r="B42" s="116" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C42" s="116"/>
       <c r="D42" s="116"/>
@@ -3537,7 +3526,7 @@
         <v>181</v>
       </c>
       <c r="B43" s="115" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D43" s="116"/>
     </row>
@@ -3546,7 +3535,7 @@
         <v>181</v>
       </c>
       <c r="B44" s="115" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C44" s="116"/>
       <c r="D44" s="116"/>
@@ -3556,7 +3545,7 @@
         <v>181</v>
       </c>
       <c r="B45" s="114" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C45" s="116"/>
       <c r="D45" s="116"/>
@@ -4024,7 +4013,7 @@
         <v>123</v>
       </c>
       <c r="G52" s="44" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H52" s="35"/>
       <c r="I52" s="36" t="s">
@@ -4043,7 +4032,7 @@
         <v>125</v>
       </c>
       <c r="N52" s="44" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="O52" s="36" t="s">
         <v>192</v>
@@ -4218,7 +4207,7 @@
         <v>192</v>
       </c>
       <c r="BU52" s="112" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="BV52" s="35">
         <v>1</v>
@@ -4253,7 +4242,7 @@
         <v>78</v>
       </c>
       <c r="K53" s="44" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L53" s="35" t="s">
         <v>79</v>
@@ -4437,7 +4426,7 @@
         <v>192</v>
       </c>
       <c r="BU53" s="112" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="BV53" s="35">
         <v>3</v>
@@ -4462,7 +4451,7 @@
         <v>133</v>
       </c>
       <c r="G54" s="53" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H54" s="35"/>
       <c r="I54" s="36" t="s">
@@ -4478,7 +4467,7 @@
         <v>79</v>
       </c>
       <c r="M54" s="53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="N54" s="35" t="s">
         <v>136</v>
@@ -4656,7 +4645,7 @@
         <v>192</v>
       </c>
       <c r="BU54" s="112" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="BV54" s="35">
         <v>1</v>
@@ -4681,7 +4670,7 @@
         <v>139</v>
       </c>
       <c r="G55" s="105" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="H55" s="35"/>
       <c r="I55" s="36" t="s">
@@ -4697,7 +4686,7 @@
         <v>79</v>
       </c>
       <c r="M55" s="105" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="N55" s="35" t="s">
         <v>141</v>
@@ -4875,7 +4864,7 @@
         <v>192</v>
       </c>
       <c r="BU55" s="112" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="BV55" s="35">
         <v>1</v>
@@ -5094,7 +5083,7 @@
         <v>192</v>
       </c>
       <c r="BU56" s="112" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="BV56" s="35">
         <v>1</v>
@@ -5119,7 +5108,7 @@
         <v>149</v>
       </c>
       <c r="G57" s="70" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H57" s="35"/>
       <c r="I57" s="36" t="s">
@@ -5313,7 +5302,7 @@
         <v>192</v>
       </c>
       <c r="BU57" s="112" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="BV57" s="35">
         <v>1</v>
@@ -6743,7 +6732,7 @@
     <row r="77" spans="1:75">
       <c r="A77" s="37"/>
       <c r="B77" s="40" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41"/>
@@ -7833,12 +7822,12 @@
     <row r="87" spans="1:75" ht="14.25">
       <c r="A87" s="38"/>
       <c r="B87" s="46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="88" spans="1:75">
       <c r="B88" s="40" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C88" s="43"/>
       <c r="D88" s="43"/>
@@ -7863,7 +7852,7 @@
         <v>6</v>
       </c>
       <c r="H89" s="33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="90" spans="1:75">
@@ -7883,7 +7872,7 @@
         <v>192</v>
       </c>
       <c r="G90" s="35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H90" s="35" t="s">
         <v>244</v>
@@ -7950,7 +7939,7 @@
         <v>192</v>
       </c>
       <c r="G93" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H93" s="35"/>
     </row>
@@ -7971,13 +7960,13 @@
         <v>192</v>
       </c>
       <c r="G94" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H94" s="35"/>
     </row>
     <row r="95" spans="1:75">
       <c r="B95" s="44" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C95" s="44" t="s">
         <v>89</v>
@@ -7992,13 +7981,13 @@
         <v>192</v>
       </c>
       <c r="G95" s="35" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H95" s="35"/>
     </row>
     <row r="96" spans="1:75">
       <c r="B96" s="44" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C96" s="44" t="s">
         <v>91</v>
@@ -8013,7 +8002,7 @@
         <v>192</v>
       </c>
       <c r="G96" s="35" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H96" s="35"/>
     </row>
@@ -8026,12 +8015,12 @@
     <row r="99" spans="1:9" ht="14.25">
       <c r="A99" s="38"/>
       <c r="B99" s="46" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="B100" s="40" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15">
@@ -8058,7 +8047,7 @@
     </row>
     <row r="102" spans="1:9">
       <c r="B102" s="44" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C102" s="44" t="s">
         <v>89</v>
@@ -8073,7 +8062,7 @@
         <v>192</v>
       </c>
       <c r="G102" s="44" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -8093,7 +8082,7 @@
         <v>192</v>
       </c>
       <c r="G103" s="44" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -8113,7 +8102,7 @@
         <v>192</v>
       </c>
       <c r="G104" s="44" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -8133,7 +8122,7 @@
         <v>192</v>
       </c>
       <c r="G105" s="44" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -8153,7 +8142,7 @@
         <v>192</v>
       </c>
       <c r="G106" s="44" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -8173,7 +8162,7 @@
         <v>192</v>
       </c>
       <c r="G107" s="44" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -8193,7 +8182,7 @@
         <v>192</v>
       </c>
       <c r="G108" s="44" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -8213,7 +8202,7 @@
         <v>192</v>
       </c>
       <c r="G109" s="44" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="15">
@@ -8233,7 +8222,7 @@
         <v>192</v>
       </c>
       <c r="G110" s="44" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -8253,7 +8242,7 @@
         <v>192</v>
       </c>
       <c r="G111" s="44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -8270,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BV17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8282,12 +8271,12 @@
         <v>86</v>
       </c>
       <c r="B2" s="100" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:74" s="80" customFormat="1" ht="12">
       <c r="B3" s="83" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C3" s="84" t="s">
         <v>87</v>
@@ -8398,7 +8387,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="105" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D5" s="105" t="s">
         <v>180</v>
@@ -8410,25 +8399,25 @@
         <v>192</v>
       </c>
       <c r="G5" s="105" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H5" s="105" t="s">
         <v>259</v>
       </c>
       <c r="I5" s="105" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J5" s="105" t="s">
         <v>259</v>
       </c>
       <c r="K5" s="105" t="s">
+        <v>428</v>
+      </c>
+      <c r="L5" s="105" t="s">
+        <v>429</v>
+      </c>
+      <c r="M5" s="105" t="s">
         <v>430</v>
-      </c>
-      <c r="L5" s="105" t="s">
-        <v>431</v>
-      </c>
-      <c r="M5" s="105" t="s">
-        <v>432</v>
       </c>
       <c r="N5" s="105" t="s">
         <v>169</v>
@@ -8458,7 +8447,7 @@
         <v>77</v>
       </c>
       <c r="W5" s="105" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X5" s="99" t="s">
         <v>192</v>
@@ -8466,17 +8455,17 @@
       <c r="Y5" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="Z5" s="105" t="s">
-        <v>248</v>
+      <c r="Z5" s="112" t="s">
+        <v>259</v>
       </c>
       <c r="AA5" s="105" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="AB5" s="105" t="s">
         <v>249</v>
       </c>
       <c r="AC5" s="105" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AD5" s="99" t="s">
         <v>192</v>
@@ -8485,7 +8474,7 @@
         <v>135</v>
       </c>
       <c r="AF5" s="105" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AG5" s="101"/>
       <c r="AH5" s="101"/>
@@ -8533,10 +8522,10 @@
     <row r="6" spans="1:74" s="102" customFormat="1">
       <c r="A6" s="100"/>
       <c r="B6" s="105" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C6" s="105" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D6" s="105" t="s">
         <v>180</v>
@@ -8548,13 +8537,13 @@
         <v>90</v>
       </c>
       <c r="G6" s="105" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H6" s="105" t="s">
         <v>260</v>
       </c>
       <c r="I6" s="105" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J6" s="99" t="s">
         <v>192</v>
@@ -8566,7 +8555,7 @@
         <v>90</v>
       </c>
       <c r="M6" s="105" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N6" s="99" t="s">
         <v>192</v>
@@ -8604,8 +8593,8 @@
       <c r="Y6" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="Z6" s="105" t="s">
-        <v>248</v>
+      <c r="Z6" s="112" t="s">
+        <v>200</v>
       </c>
       <c r="AA6" s="99" t="s">
         <v>90</v>
@@ -8671,10 +8660,10 @@
     <row r="7" spans="1:74" s="102" customFormat="1">
       <c r="A7" s="100"/>
       <c r="B7" s="105" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C7" s="105" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D7" s="105" t="s">
         <v>180</v>
@@ -8686,7 +8675,7 @@
         <v>90</v>
       </c>
       <c r="G7" s="105" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H7" s="105" t="s">
         <v>259</v>
@@ -8704,7 +8693,7 @@
         <v>90</v>
       </c>
       <c r="M7" s="105" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N7" s="99" t="s">
         <v>192</v>
@@ -8742,8 +8731,8 @@
       <c r="Y7" s="105" t="s">
         <v>192</v>
       </c>
-      <c r="Z7" s="105" t="s">
-        <v>248</v>
+      <c r="Z7" s="112" t="s">
+        <v>259</v>
       </c>
       <c r="AA7" s="99" t="s">
         <v>90</v>
@@ -8809,10 +8798,10 @@
     <row r="8" spans="1:74" s="102" customFormat="1">
       <c r="A8" s="100"/>
       <c r="B8" s="105" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C8" s="105" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D8" s="105" t="s">
         <v>180</v>
@@ -8824,13 +8813,13 @@
         <v>192</v>
       </c>
       <c r="G8" s="105" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H8" s="105" t="s">
         <v>260</v>
       </c>
       <c r="I8" s="105" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J8" s="105" t="s">
         <v>249</v>
@@ -8848,13 +8837,13 @@
         <v>254</v>
       </c>
       <c r="O8" s="105" t="s">
+        <v>399</v>
+      </c>
+      <c r="P8" s="105" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q8" s="105" t="s">
         <v>401</v>
-      </c>
-      <c r="P8" s="105" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q8" s="105" t="s">
-        <v>403</v>
       </c>
       <c r="R8" s="105" t="s">
         <v>207</v>
@@ -8880,8 +8869,8 @@
       <c r="Y8" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="Z8" s="105" t="s">
-        <v>248</v>
+      <c r="Z8" s="112" t="s">
+        <v>259</v>
       </c>
       <c r="AA8" s="99" t="s">
         <v>90</v>
@@ -8890,7 +8879,7 @@
         <v>90</v>
       </c>
       <c r="AC8" s="105" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="AD8" s="99" t="s">
         <v>90</v>
@@ -8899,7 +8888,7 @@
         <v>90</v>
       </c>
       <c r="AF8" s="105" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AG8" s="101"/>
       <c r="AH8" s="101"/>
@@ -8950,50 +8939,50 @@
         <v>201</v>
       </c>
       <c r="C9" s="112" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D9" s="112" t="s">
         <v>180</v>
       </c>
       <c r="E9" s="110" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="F9" s="108" t="s">
         <v>192</v>
       </c>
       <c r="G9" s="110" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H9" s="110" t="s">
         <v>271</v>
       </c>
       <c r="I9" s="110" t="s">
+        <v>523</v>
+      </c>
+      <c r="J9" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="K9" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="L9" s="110" t="s">
+        <v>376</v>
+      </c>
+      <c r="M9" s="110" t="s">
+        <v>378</v>
+      </c>
+      <c r="N9" s="110" t="s">
+        <v>524</v>
+      </c>
+      <c r="O9" s="110" t="s">
+        <v>525</v>
+      </c>
+      <c r="P9" s="110" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q9" s="110" t="s">
         <v>527</v>
       </c>
-      <c r="J9" s="108" t="s">
-        <v>192</v>
-      </c>
-      <c r="K9" s="108" t="s">
-        <v>192</v>
-      </c>
-      <c r="L9" s="110" t="s">
-        <v>378</v>
-      </c>
-      <c r="M9" s="110" t="s">
-        <v>380</v>
-      </c>
-      <c r="N9" s="110" t="s">
-        <v>528</v>
-      </c>
-      <c r="O9" s="110" t="s">
-        <v>529</v>
-      </c>
-      <c r="P9" s="110" t="s">
-        <v>530</v>
-      </c>
-      <c r="Q9" s="110" t="s">
-        <v>531</v>
-      </c>
       <c r="R9" s="108" t="s">
         <v>192</v>
       </c>
@@ -9004,22 +8993,22 @@
         <v>192</v>
       </c>
       <c r="U9" s="110" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="V9" s="110" t="s">
         <v>200</v>
       </c>
       <c r="W9" s="110" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="X9" s="108" t="s">
         <v>192</v>
       </c>
       <c r="Y9" s="110" t="s">
-        <v>532</v>
-      </c>
-      <c r="Z9" s="110" t="s">
-        <v>447</v>
+        <v>528</v>
+      </c>
+      <c r="Z9" s="112" t="s">
+        <v>200</v>
       </c>
       <c r="AA9" s="108" t="s">
         <v>90</v>
@@ -9034,7 +9023,7 @@
         <v>90</v>
       </c>
       <c r="AE9" s="110" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="AF9" s="108" t="s">
         <v>90</v>
@@ -9088,7 +9077,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="100" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="100"/>
@@ -9163,7 +9152,7 @@
     </row>
     <row r="12" spans="1:74" s="80" customFormat="1" ht="12">
       <c r="B12" s="83" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:74" s="80" customFormat="1" ht="12">
@@ -9171,10 +9160,10 @@
         <v>256</v>
       </c>
       <c r="C13" s="92" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D13" s="92" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:74" s="80" customFormat="1" ht="12">
@@ -9185,12 +9174,12 @@
         <v>271</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:74" s="102" customFormat="1">
       <c r="B15" s="112" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C15" s="112" t="s">
         <v>201</v>
@@ -9201,13 +9190,13 @@
     </row>
     <row r="16" spans="1:74" s="102" customFormat="1">
       <c r="B16" s="112" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C16" s="112" t="s">
         <v>201</v>
       </c>
       <c r="D16" s="112" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17" s="111" customFormat="1" ht="12"/>
@@ -9221,8 +9210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9266,7 +9255,7 @@
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="75" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>250</v>
@@ -9281,7 +9270,7 @@
         <v>253</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K5" s="75"/>
       <c r="L5" s="75"/>
@@ -9289,16 +9278,16 @@
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="75" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="I6" s="26" t="s">
         <v>274</v>
@@ -9309,11 +9298,11 @@
     </row>
     <row r="7" spans="2:13" s="9" customFormat="1">
       <c r="B7" s="75" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="75" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E7" s="75"/>
       <c r="F7" s="18"/>
@@ -9328,17 +9317,17 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="75" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="75" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="I8" s="26" t="s">
         <v>275</v>
@@ -9349,17 +9338,17 @@
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="75" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="75" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I9" s="26" t="s">
         <v>276</v>
@@ -9412,10 +9401,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H197"/>
+  <dimension ref="A1:H195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9464,7 +9453,7 @@
         <v>325</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>304</v>
@@ -9479,7 +9468,7 @@
         <v>326</v>
       </c>
       <c r="C6" s="87" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>305</v>
@@ -9510,7 +9499,7 @@
         <v>328</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>302</v>
@@ -9525,7 +9514,7 @@
         <v>329</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>318</v>
@@ -9540,10 +9529,10 @@
         <v>330</v>
       </c>
       <c r="C10" s="87" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25">
@@ -9554,7 +9543,7 @@
         <v>331</v>
       </c>
       <c r="C11" s="87" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>308</v>
@@ -9582,7 +9571,7 @@
         <v>333</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>317</v>
@@ -9610,7 +9599,7 @@
         <v>335</v>
       </c>
       <c r="C15" s="87" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>312</v>
@@ -9621,10 +9610,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C16" s="87" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>313</v>
@@ -9638,7 +9627,7 @@
         <v>336</v>
       </c>
       <c r="C17" s="87" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>303</v>
@@ -9652,10 +9641,10 @@
         <v>337</v>
       </c>
       <c r="C18" s="87" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.25">
@@ -9666,10 +9655,10 @@
         <v>338</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.25">
@@ -9778,10 +9767,10 @@
         <v>346</v>
       </c>
       <c r="C27" s="87" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.25">
@@ -9789,10 +9778,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C28" s="87" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>311</v>
@@ -9871,7 +9860,7 @@
         <v>325</v>
       </c>
       <c r="C44" s="87" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D44" s="49" t="s">
         <v>304</v>
@@ -9886,7 +9875,7 @@
         <v>326</v>
       </c>
       <c r="C45" s="87" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D45" s="49" t="s">
         <v>305</v>
@@ -9901,7 +9890,7 @@
         <v>328</v>
       </c>
       <c r="C46" s="87" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>302</v>
@@ -9916,7 +9905,7 @@
         <v>329</v>
       </c>
       <c r="C47" s="87" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>318</v>
@@ -9931,10 +9920,10 @@
         <v>330</v>
       </c>
       <c r="C48" s="87" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="52" customFormat="1" ht="14.25">
@@ -9945,7 +9934,7 @@
         <v>331</v>
       </c>
       <c r="C49" s="87" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D49" s="49" t="s">
         <v>308</v>
@@ -9973,7 +9962,7 @@
         <v>333</v>
       </c>
       <c r="C51" s="87" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D51" s="49" t="s">
         <v>317</v>
@@ -10001,7 +9990,7 @@
         <v>335</v>
       </c>
       <c r="C53" s="87" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D53" s="87" t="s">
         <v>312</v>
@@ -10012,10 +10001,10 @@
         <v>4</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C54" s="87" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D54" s="48" t="s">
         <v>313</v>
@@ -10029,7 +10018,7 @@
         <v>336</v>
       </c>
       <c r="C55" s="87" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D55" s="48" t="s">
         <v>303</v>
@@ -10043,10 +10032,10 @@
         <v>337</v>
       </c>
       <c r="C56" s="87" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="52" customFormat="1" ht="14.25">
@@ -10057,10 +10046,10 @@
         <v>338</v>
       </c>
       <c r="C57" s="87" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="52" customFormat="1" ht="14.25">
@@ -10172,7 +10161,7 @@
         <v>18</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="52" customFormat="1" ht="14.25">
@@ -10180,10 +10169,10 @@
         <v>4</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C66" s="87" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D66" s="48" t="s">
         <v>311</v>
@@ -10197,304 +10186,300 @@
         <v>347</v>
       </c>
       <c r="C67" s="87" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D67" s="48" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="52" customFormat="1" ht="14.25">
-      <c r="A68" s="47"/>
-      <c r="B68" s="50" t="s">
-        <v>347</v>
-      </c>
-      <c r="C68" s="87" t="s">
-        <v>351</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>320</v>
-      </c>
-    </row>
+    <row r="68" spans="1:6" s="52" customFormat="1"/>
     <row r="69" spans="1:6" s="52" customFormat="1" ht="14.25">
-      <c r="A69" s="47"/>
-      <c r="B69" s="50" t="s">
-        <v>347</v>
-      </c>
-      <c r="C69" s="87" t="s">
-        <v>353</v>
-      </c>
-      <c r="D69" s="48" t="s">
-        <v>320</v>
+      <c r="A69" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="52" t="s">
+        <v>321</v>
+      </c>
+      <c r="C69" s="52" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="52" customFormat="1"/>
-    <row r="71" spans="1:6" s="52" customFormat="1" ht="14.25">
-      <c r="A71" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" s="52" t="s">
-        <v>321</v>
-      </c>
-      <c r="C71" s="52" t="s">
-        <v>247</v>
-      </c>
-    </row>
+    <row r="71" spans="1:6" s="52" customFormat="1"/>
     <row r="72" spans="1:6" s="52" customFormat="1"/>
-    <row r="73" spans="1:6" s="52" customFormat="1"/>
-    <row r="74" spans="1:6" s="52" customFormat="1"/>
+    <row r="73" spans="1:6" s="54" customFormat="1" ht="14.25">
+      <c r="A73" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="56" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="54" customFormat="1"/>
     <row r="75" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A75" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B75" s="56" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="54" customFormat="1"/>
-    <row r="77" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A77" s="61"/>
-      <c r="B77" s="57" t="s">
+      <c r="A75" s="61"/>
+      <c r="B75" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="57" t="s">
+      <c r="C75" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="57" t="s">
+      <c r="D75" s="57" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="76" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="A76" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B76" s="64" t="s">
+        <v>325</v>
+      </c>
+      <c r="C76" s="87" t="s">
+        <v>420</v>
+      </c>
+      <c r="D76" s="63" t="s">
+        <v>304</v>
+      </c>
+      <c r="F76" s="58"/>
+    </row>
+    <row r="77" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="A77" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="64" t="s">
+        <v>326</v>
+      </c>
+      <c r="C77" s="87" t="s">
+        <v>421</v>
+      </c>
+      <c r="D77" s="63" t="s">
+        <v>305</v>
+      </c>
+      <c r="F77" s="58"/>
     </row>
     <row r="78" spans="1:6" s="54" customFormat="1" ht="15">
       <c r="A78" s="61" t="s">
-        <v>202</v>
+        <v>4</v>
       </c>
       <c r="B78" s="64" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C78" s="87" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="D78" s="63" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F78" s="58"/>
     </row>
     <row r="79" spans="1:6" s="54" customFormat="1" ht="15">
       <c r="A79" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B79" s="64" t="s">
+        <v>329</v>
+      </c>
+      <c r="C79" s="87" t="s">
+        <v>355</v>
+      </c>
+      <c r="D79" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="F79" s="58"/>
+    </row>
+    <row r="80" spans="1:6" s="74" customFormat="1" ht="14.25">
+      <c r="A80" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="64" t="s">
-        <v>326</v>
-      </c>
-      <c r="C79" s="87" t="s">
-        <v>423</v>
-      </c>
-      <c r="D79" s="63" t="s">
-        <v>305</v>
-      </c>
-      <c r="F79" s="58"/>
-    </row>
-    <row r="80" spans="1:6" s="54" customFormat="1" ht="15">
-      <c r="A80" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="64" t="s">
-        <v>328</v>
-      </c>
-      <c r="C80" s="87" t="s">
-        <v>436</v>
-      </c>
-      <c r="D80" s="63" t="s">
-        <v>302</v>
-      </c>
-      <c r="F80" s="58"/>
-    </row>
-    <row r="81" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="B80" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C80" s="87">
+        <v>13900000000</v>
+      </c>
+      <c r="D80" s="88" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A81" s="61" t="s">
         <v>202</v>
       </c>
       <c r="B81" s="64" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="C81" s="87" t="s">
-        <v>357</v>
-      </c>
-      <c r="D81" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="F81" s="58"/>
-    </row>
-    <row r="82" spans="1:6" s="74" customFormat="1" ht="14.25">
-      <c r="A82" s="85" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="89" t="s">
-        <v>331</v>
-      </c>
-      <c r="C82" s="87">
-        <v>13900000000</v>
-      </c>
-      <c r="D82" s="88" t="s">
-        <v>308</v>
-      </c>
-    </row>
+        <v>424</v>
+      </c>
+      <c r="D81" s="62" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="54" customFormat="1"/>
     <row r="83" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A83" s="61" t="s">
-        <v>202</v>
-      </c>
-      <c r="B83" s="64" t="s">
-        <v>338</v>
-      </c>
-      <c r="C83" s="87" t="s">
-        <v>426</v>
-      </c>
-      <c r="D83" s="62" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="54" customFormat="1"/>
+        <v>18</v>
+      </c>
+      <c r="B83" s="54" t="s">
+        <v>321</v>
+      </c>
+      <c r="C83" s="54" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="14.25">
+      <c r="A84" s="61"/>
+      <c r="B84" s="56"/>
+    </row>
     <row r="85" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A85" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B85" s="54" t="s">
-        <v>321</v>
-      </c>
-      <c r="C85" s="54" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="14.25">
-      <c r="A86" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="56" t="s">
-        <v>307</v>
-      </c>
-    </row>
+      <c r="A85" s="61"/>
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="1:6" s="54" customFormat="1" ht="12.75" customHeight="1"/>
     <row r="87" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A87" s="61" t="s">
-        <v>445</v>
-      </c>
-      <c r="B87" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" s="54" customFormat="1" ht="12.75" customHeight="1"/>
+        <v>0</v>
+      </c>
+      <c r="B87" s="56" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="54" customFormat="1"/>
     <row r="89" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A89" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="56" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" s="54" customFormat="1"/>
-    <row r="91" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A91" s="61"/>
-      <c r="B91" s="57" t="s">
+      <c r="A89" s="61"/>
+      <c r="B89" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="57" t="s">
+      <c r="C89" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="57" t="s">
+      <c r="D89" s="57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="54" customFormat="1" ht="15">
+    <row r="90" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="A90" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="64" t="s">
+        <v>328</v>
+      </c>
+      <c r="C90" s="87" t="s">
+        <v>436</v>
+      </c>
+      <c r="D90" s="63" t="s">
+        <v>302</v>
+      </c>
+      <c r="F90" s="58"/>
+    </row>
+    <row r="91" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="A91" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B91" s="64" t="s">
+        <v>329</v>
+      </c>
+      <c r="C91" s="87" t="s">
+        <v>435</v>
+      </c>
+      <c r="D91" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="F91" s="58"/>
+    </row>
+    <row r="92" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A92" s="61" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
       <c r="B92" s="64" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C92" s="87" t="s">
-        <v>438</v>
-      </c>
-      <c r="D92" s="63" t="s">
-        <v>302</v>
-      </c>
-      <c r="F92" s="58"/>
-    </row>
-    <row r="93" spans="1:6" s="54" customFormat="1" ht="15">
-      <c r="A93" s="61" t="s">
-        <v>202</v>
-      </c>
-      <c r="B93" s="64" t="s">
-        <v>329</v>
-      </c>
-      <c r="C93" s="87" t="s">
-        <v>437</v>
-      </c>
-      <c r="D93" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="F93" s="58"/>
-    </row>
+        <v>430</v>
+      </c>
+      <c r="D92" s="62" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="54" customFormat="1"/>
     <row r="94" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A94" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="54" t="s">
+        <v>321</v>
+      </c>
+      <c r="C94" s="54" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="54" customFormat="1"/>
+    <row r="96" spans="1:6" s="54" customFormat="1"/>
+    <row r="99" spans="1:6" s="54" customFormat="1" ht="14.25">
+      <c r="A99" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="56" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="54" customFormat="1"/>
+    <row r="101" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="A101" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="B94" s="64" t="s">
-        <v>338</v>
-      </c>
-      <c r="C94" s="87" t="s">
-        <v>432</v>
-      </c>
-      <c r="D94" s="62" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" s="54" customFormat="1"/>
-    <row r="96" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A96" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B96" s="54" t="s">
-        <v>321</v>
-      </c>
-      <c r="C96" s="54" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" s="54" customFormat="1"/>
-    <row r="98" spans="1:6" s="54" customFormat="1"/>
-    <row r="101" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A101" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B101" s="56" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" s="54" customFormat="1"/>
-    <row r="103" spans="1:6" s="54" customFormat="1" ht="15">
+      <c r="B101" s="64" t="s">
+        <v>325</v>
+      </c>
+      <c r="C101" s="87" t="s">
+        <v>134</v>
+      </c>
+      <c r="D101" s="63" t="s">
+        <v>304</v>
+      </c>
+      <c r="F101" s="58"/>
+    </row>
+    <row r="102" spans="1:6" s="54" customFormat="1" ht="14.25">
+      <c r="A102" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="64" t="s">
+        <v>339</v>
+      </c>
+      <c r="C102" s="87">
+        <v>5</v>
+      </c>
+      <c r="D102" s="62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A103" s="61" t="s">
-        <v>202</v>
+        <v>4</v>
       </c>
       <c r="B103" s="64" t="s">
-        <v>325</v>
-      </c>
-      <c r="C103" s="87" t="s">
-        <v>134</v>
-      </c>
-      <c r="D103" s="63" t="s">
-        <v>304</v>
-      </c>
-      <c r="F103" s="58"/>
+        <v>340</v>
+      </c>
+      <c r="C103" s="87">
+        <v>6</v>
+      </c>
+      <c r="D103" s="62" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="104" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A104" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B104" s="64" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C104" s="87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D104" s="62" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="105" spans="1:6" s="54" customFormat="1" ht="14.25">
@@ -10502,13 +10487,13 @@
         <v>4</v>
       </c>
       <c r="B105" s="64" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C105" s="87">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D105" s="62" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="54" customFormat="1" ht="14.25">
@@ -10516,27 +10501,27 @@
         <v>4</v>
       </c>
       <c r="B106" s="64" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C106" s="87">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D106" s="62" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A107" s="61" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
       <c r="B107" s="64" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C107" s="87">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D107" s="62" t="s">
-        <v>162</v>
+        <v>315</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="54" customFormat="1" ht="14.25">
@@ -10544,66 +10529,56 @@
         <v>4</v>
       </c>
       <c r="B108" s="64" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C108" s="87">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D108" s="62" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A109" s="61" t="s">
-        <v>202</v>
-      </c>
-      <c r="B109" s="64" t="s">
-        <v>344</v>
-      </c>
-      <c r="C109" s="87">
-        <v>10</v>
-      </c>
-      <c r="D109" s="62" t="s">
-        <v>315</v>
-      </c>
-    </row>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="54" customFormat="1"/>
     <row r="110" spans="1:6" s="54" customFormat="1" ht="14.25">
       <c r="A110" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="64" t="s">
-        <v>345</v>
-      </c>
-      <c r="C110" s="87">
-        <v>11</v>
-      </c>
-      <c r="D110" s="62" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" s="54" customFormat="1"/>
-    <row r="112" spans="1:6" s="54" customFormat="1" ht="14.25">
-      <c r="A112" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B112" s="54" t="s">
+      <c r="B110" s="54" t="s">
         <v>321</v>
       </c>
-      <c r="C112" s="54" t="s">
+      <c r="C110" s="54" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="113" spans="1:2" s="54" customFormat="1" ht="14.25">
-      <c r="A113" s="19" t="s">
+    <row r="111" spans="1:6" s="54" customFormat="1" ht="14.25">
+      <c r="A111" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B113" s="25" t="s">
+      <c r="B111" s="25" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="54" customFormat="1"/>
-    <row r="115" spans="1:2" s="54" customFormat="1"/>
+    <row r="112" spans="1:6" s="54" customFormat="1"/>
+    <row r="113" s="54" customFormat="1"/>
+    <row r="188" spans="1:7">
+      <c r="C188" s="14"/>
+      <c r="D188" s="14"/>
+      <c r="E188" s="14"/>
+      <c r="F188" s="14"/>
+      <c r="G188" s="14"/>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" s="14"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="14"/>
+      <c r="D189" s="14"/>
+      <c r="E189" s="14"/>
+      <c r="F189" s="14"/>
+      <c r="G189" s="14"/>
+    </row>
     <row r="190" spans="1:7">
+      <c r="A190" s="14"/>
+      <c r="B190" s="14"/>
       <c r="C190" s="14"/>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
@@ -10642,28 +10617,10 @@
       <c r="B194" s="14"/>
       <c r="C194" s="14"/>
       <c r="D194" s="14"/>
-      <c r="E194" s="14"/>
-      <c r="F194" s="14"/>
-      <c r="G194" s="14"/>
     </row>
     <row r="195" spans="1:7">
       <c r="A195" s="14"/>
       <c r="B195" s="14"/>
-      <c r="C195" s="14"/>
-      <c r="D195" s="14"/>
-      <c r="E195" s="14"/>
-      <c r="F195" s="14"/>
-      <c r="G195" s="14"/>
-    </row>
-    <row r="196" spans="1:7">
-      <c r="A196" s="14"/>
-      <c r="B196" s="14"/>
-      <c r="C196" s="14"/>
-      <c r="D196" s="14"/>
-    </row>
-    <row r="197" spans="1:7">
-      <c r="A197" s="14"/>
-      <c r="B197" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -10680,8 +10637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BV17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5:Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -10707,12 +10664,12 @@
         <v>86</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:74" s="60" customFormat="1">
       <c r="B3" s="69" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>87</v>
@@ -10823,7 +10780,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D5" s="70" t="s">
         <v>180</v>
@@ -10835,25 +10792,25 @@
         <v>90</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H5" s="70" t="s">
         <v>260</v>
       </c>
       <c r="I5" s="70" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J5" s="70" t="s">
         <v>260</v>
       </c>
       <c r="K5" s="70" t="s">
+        <v>396</v>
+      </c>
+      <c r="L5" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="M5" s="70" t="s">
         <v>398</v>
-      </c>
-      <c r="L5" s="70" t="s">
-        <v>399</v>
-      </c>
-      <c r="M5" s="70" t="s">
-        <v>400</v>
       </c>
       <c r="N5" s="70" t="s">
         <v>249</v>
@@ -10862,13 +10819,13 @@
         <v>254</v>
       </c>
       <c r="P5" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q5" s="70" t="s">
+        <v>400</v>
+      </c>
+      <c r="R5" s="70" t="s">
         <v>401</v>
-      </c>
-      <c r="Q5" s="70" t="s">
-        <v>402</v>
-      </c>
-      <c r="R5" s="70" t="s">
-        <v>403</v>
       </c>
       <c r="S5" s="70" t="s">
         <v>207</v>
@@ -10877,13 +10834,13 @@
         <v>169</v>
       </c>
       <c r="U5" s="70" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="V5" s="70" t="s">
         <v>259</v>
       </c>
       <c r="W5" s="70" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X5" s="95" t="s">
         <v>90</v>
@@ -10891,26 +10848,26 @@
       <c r="Y5" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="Z5" s="70" t="s">
-        <v>248</v>
+      <c r="Z5" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA5" s="103" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="AB5" s="70" t="s">
         <v>248</v>
       </c>
       <c r="AC5" s="70" t="s">
+        <v>404</v>
+      </c>
+      <c r="AD5" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" s="70" t="s">
+        <v>405</v>
+      </c>
+      <c r="AF5" s="70" t="s">
         <v>406</v>
-      </c>
-      <c r="AD5" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE5" s="70" t="s">
-        <v>407</v>
-      </c>
-      <c r="AF5" s="70" t="s">
-        <v>408</v>
       </c>
       <c r="AG5" s="65"/>
       <c r="AH5" s="65"/>
@@ -10961,7 +10918,7 @@
         <v>260</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D6" s="70" t="s">
         <v>180</v>
@@ -10973,25 +10930,25 @@
         <v>192</v>
       </c>
       <c r="G6" s="94" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H6" s="94" t="s">
         <v>259</v>
       </c>
       <c r="I6" s="94" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J6" s="94" t="s">
         <v>259</v>
       </c>
       <c r="K6" s="94" t="s">
+        <v>428</v>
+      </c>
+      <c r="L6" s="94" t="s">
+        <v>429</v>
+      </c>
+      <c r="M6" s="94" t="s">
         <v>430</v>
-      </c>
-      <c r="L6" s="94" t="s">
-        <v>431</v>
-      </c>
-      <c r="M6" s="94" t="s">
-        <v>432</v>
       </c>
       <c r="N6" s="94" t="s">
         <v>169</v>
@@ -11021,7 +10978,7 @@
         <v>77</v>
       </c>
       <c r="W6" s="94" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X6" s="95" t="s">
         <v>192</v>
@@ -11029,17 +10986,17 @@
       <c r="Y6" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="Z6" s="94" t="s">
-        <v>248</v>
+      <c r="Z6" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA6" s="103" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="AB6" s="94" t="s">
         <v>249</v>
       </c>
       <c r="AC6" s="94" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AD6" s="95" t="s">
         <v>192</v>
@@ -11048,7 +11005,7 @@
         <v>135</v>
       </c>
       <c r="AF6" s="94" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AG6" s="65"/>
       <c r="AH6" s="65"/>
@@ -11096,10 +11053,10 @@
     <row r="7" spans="1:74" s="54" customFormat="1" ht="13.5">
       <c r="A7" s="72"/>
       <c r="B7" s="70" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D7" s="70" t="s">
         <v>180</v>
@@ -11111,13 +11068,13 @@
         <v>90</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H7" s="94" t="s">
         <v>260</v>
       </c>
       <c r="I7" s="94" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J7" s="95" t="s">
         <v>192</v>
@@ -11129,7 +11086,7 @@
         <v>90</v>
       </c>
       <c r="M7" s="94" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N7" s="95" t="s">
         <v>192</v>
@@ -11167,8 +11124,8 @@
       <c r="Y7" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="Z7" s="94" t="s">
-        <v>248</v>
+      <c r="Z7" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA7" s="95" t="s">
         <v>90</v>
@@ -11234,10 +11191,10 @@
     <row r="8" spans="1:74" s="54" customFormat="1" ht="13.5">
       <c r="A8" s="72"/>
       <c r="B8" s="70" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D8" s="70" t="s">
         <v>180</v>
@@ -11249,7 +11206,7 @@
         <v>90</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H8" s="94" t="s">
         <v>259</v>
@@ -11267,7 +11224,7 @@
         <v>90</v>
       </c>
       <c r="M8" s="94" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N8" s="95" t="s">
         <v>192</v>
@@ -11305,8 +11262,8 @@
       <c r="Y8" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="Z8" s="94" t="s">
-        <v>248</v>
+      <c r="Z8" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA8" s="95" t="s">
         <v>90</v>
@@ -11372,10 +11329,10 @@
     <row r="9" spans="1:74" s="54" customFormat="1" ht="13.5">
       <c r="A9" s="72"/>
       <c r="B9" s="70" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D9" s="70" t="s">
         <v>180</v>
@@ -11414,13 +11371,13 @@
         <v>254</v>
       </c>
       <c r="P9" s="94" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q9" s="94" t="s">
+        <v>400</v>
+      </c>
+      <c r="R9" s="94" t="s">
         <v>401</v>
-      </c>
-      <c r="Q9" s="94" t="s">
-        <v>402</v>
-      </c>
-      <c r="R9" s="94" t="s">
-        <v>403</v>
       </c>
       <c r="S9" s="94" t="s">
         <v>207</v>
@@ -11443,8 +11400,8 @@
       <c r="Y9" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="Z9" s="94" t="s">
-        <v>248</v>
+      <c r="Z9" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA9" s="95" t="s">
         <v>192</v>
@@ -11513,7 +11470,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E11" s="72"/>
       <c r="F11" s="72"/>
@@ -11588,7 +11545,7 @@
     </row>
     <row r="12" spans="1:74" s="60" customFormat="1">
       <c r="B12" s="69" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:74" s="60" customFormat="1">
@@ -11596,10 +11553,10 @@
         <v>256</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:74" s="60" customFormat="1">
@@ -11621,7 +11578,7 @@
         <v>271</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:74" s="54" customFormat="1" ht="13.5"/>
@@ -11673,7 +11630,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25">
@@ -11681,7 +11638,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="80" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -11739,7 +11696,7 @@
         <v>328</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D8" s="88" t="s">
         <v>302</v>
@@ -11754,7 +11711,7 @@
         <v>329</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D9" s="88" t="s">
         <v>318</v>
@@ -11769,10 +11726,10 @@
         <v>330</v>
       </c>
       <c r="C10" s="87" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D10" s="88" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="54" customFormat="1" ht="14.25">
@@ -11783,7 +11740,7 @@
         <v>331</v>
       </c>
       <c r="C11" s="87" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D11" s="88" t="s">
         <v>308</v>
@@ -11933,7 +11890,7 @@
         <v>246</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="54" customFormat="1"/>
@@ -11949,8 +11906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BV19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE39" sqref="AE39"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5:Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11961,12 +11918,12 @@
         <v>86</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:74" s="60" customFormat="1" ht="12">
       <c r="B3" s="69" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>87</v>
@@ -12077,7 +12034,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="94" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D5" s="94" t="s">
         <v>180</v>
@@ -12089,25 +12046,25 @@
         <v>90</v>
       </c>
       <c r="G5" s="94" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H5" s="94" t="s">
         <v>260</v>
       </c>
       <c r="I5" s="94" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J5" s="94" t="s">
         <v>260</v>
       </c>
       <c r="K5" s="94" t="s">
+        <v>396</v>
+      </c>
+      <c r="L5" s="94" t="s">
+        <v>397</v>
+      </c>
+      <c r="M5" s="94" t="s">
         <v>398</v>
-      </c>
-      <c r="L5" s="94" t="s">
-        <v>399</v>
-      </c>
-      <c r="M5" s="94" t="s">
-        <v>400</v>
       </c>
       <c r="N5" s="94" t="s">
         <v>249</v>
@@ -12116,13 +12073,13 @@
         <v>254</v>
       </c>
       <c r="P5" s="94" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q5" s="94" t="s">
+        <v>400</v>
+      </c>
+      <c r="R5" s="94" t="s">
         <v>401</v>
-      </c>
-      <c r="Q5" s="94" t="s">
-        <v>402</v>
-      </c>
-      <c r="R5" s="94" t="s">
-        <v>403</v>
       </c>
       <c r="S5" s="94" t="s">
         <v>207</v>
@@ -12131,13 +12088,13 @@
         <v>169</v>
       </c>
       <c r="U5" s="94" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="V5" s="94" t="s">
         <v>259</v>
       </c>
       <c r="W5" s="94" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X5" s="95" t="s">
         <v>90</v>
@@ -12145,26 +12102,26 @@
       <c r="Y5" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="Z5" s="94" t="s">
-        <v>248</v>
+      <c r="Z5" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA5" s="105" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="AB5" s="94" t="s">
         <v>248</v>
       </c>
       <c r="AC5" s="94" t="s">
+        <v>404</v>
+      </c>
+      <c r="AD5" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE5" s="94" t="s">
+        <v>405</v>
+      </c>
+      <c r="AF5" s="94" t="s">
         <v>406</v>
-      </c>
-      <c r="AD5" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE5" s="94" t="s">
-        <v>407</v>
-      </c>
-      <c r="AF5" s="94" t="s">
-        <v>408</v>
       </c>
       <c r="AG5" s="97"/>
       <c r="AH5" s="97"/>
@@ -12215,7 +12172,7 @@
         <v>260</v>
       </c>
       <c r="C6" s="94" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D6" s="94" t="s">
         <v>180</v>
@@ -12227,25 +12184,25 @@
         <v>192</v>
       </c>
       <c r="G6" s="94" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H6" s="94" t="s">
         <v>259</v>
       </c>
       <c r="I6" s="94" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J6" s="94" t="s">
         <v>259</v>
       </c>
       <c r="K6" s="94" t="s">
+        <v>428</v>
+      </c>
+      <c r="L6" s="94" t="s">
+        <v>429</v>
+      </c>
+      <c r="M6" s="94" t="s">
         <v>430</v>
-      </c>
-      <c r="L6" s="94" t="s">
-        <v>431</v>
-      </c>
-      <c r="M6" s="94" t="s">
-        <v>432</v>
       </c>
       <c r="N6" s="94" t="s">
         <v>169</v>
@@ -12275,7 +12232,7 @@
         <v>77</v>
       </c>
       <c r="W6" s="94" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X6" s="95" t="s">
         <v>192</v>
@@ -12283,17 +12240,17 @@
       <c r="Y6" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="Z6" s="94" t="s">
-        <v>248</v>
+      <c r="Z6" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA6" s="105" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="AB6" s="94" t="s">
         <v>249</v>
       </c>
       <c r="AC6" s="94" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AD6" s="95" t="s">
         <v>192</v>
@@ -12302,7 +12259,7 @@
         <v>135</v>
       </c>
       <c r="AF6" s="94" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AG6" s="97"/>
       <c r="AH6" s="97"/>
@@ -12350,10 +12307,10 @@
     <row r="7" spans="1:74" s="90" customFormat="1">
       <c r="A7" s="96"/>
       <c r="B7" s="94" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C7" s="94" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D7" s="94" t="s">
         <v>180</v>
@@ -12365,13 +12322,13 @@
         <v>90</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H7" s="94" t="s">
         <v>260</v>
       </c>
       <c r="I7" s="94" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J7" s="95" t="s">
         <v>192</v>
@@ -12383,7 +12340,7 @@
         <v>90</v>
       </c>
       <c r="M7" s="94" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N7" s="95" t="s">
         <v>192</v>
@@ -12421,8 +12378,8 @@
       <c r="Y7" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="Z7" s="94" t="s">
-        <v>248</v>
+      <c r="Z7" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA7" s="95" t="s">
         <v>90</v>
@@ -12488,10 +12445,10 @@
     <row r="8" spans="1:74" s="90" customFormat="1">
       <c r="A8" s="96"/>
       <c r="B8" s="94" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C8" s="94" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D8" s="94" t="s">
         <v>180</v>
@@ -12503,7 +12460,7 @@
         <v>90</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H8" s="94" t="s">
         <v>259</v>
@@ -12521,7 +12478,7 @@
         <v>90</v>
       </c>
       <c r="M8" s="94" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N8" s="95" t="s">
         <v>192</v>
@@ -12559,8 +12516,8 @@
       <c r="Y8" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="Z8" s="94" t="s">
-        <v>248</v>
+      <c r="Z8" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA8" s="95" t="s">
         <v>90</v>
@@ -12626,10 +12583,10 @@
     <row r="9" spans="1:74" s="90" customFormat="1">
       <c r="A9" s="100"/>
       <c r="B9" s="98" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C9" s="98" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D9" s="98" t="s">
         <v>180</v>
@@ -12641,13 +12598,13 @@
         <v>192</v>
       </c>
       <c r="G9" s="98" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H9" s="98" t="s">
         <v>260</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J9" s="98" t="s">
         <v>249</v>
@@ -12665,13 +12622,13 @@
         <v>254</v>
       </c>
       <c r="O9" s="98" t="s">
+        <v>399</v>
+      </c>
+      <c r="P9" s="98" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q9" s="98" t="s">
         <v>401</v>
-      </c>
-      <c r="P9" s="98" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q9" s="98" t="s">
-        <v>403</v>
       </c>
       <c r="R9" s="98" t="s">
         <v>207</v>
@@ -12697,8 +12654,8 @@
       <c r="Y9" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="Z9" s="98" t="s">
-        <v>248</v>
+      <c r="Z9" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA9" s="99" t="s">
         <v>90</v>
@@ -12707,7 +12664,7 @@
         <v>90</v>
       </c>
       <c r="AC9" s="98" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="AD9" s="99" t="s">
         <v>90</v>
@@ -12716,7 +12673,7 @@
         <v>90</v>
       </c>
       <c r="AF9" s="98" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AG9" s="101"/>
       <c r="AH9" s="101"/>
@@ -12766,7 +12723,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E11" s="72"/>
       <c r="F11" s="72"/>
@@ -12841,7 +12798,7 @@
     </row>
     <row r="12" spans="1:74" s="60" customFormat="1" ht="12">
       <c r="B12" s="69" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:74" s="60" customFormat="1" ht="12">
@@ -12849,10 +12806,10 @@
         <v>256</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:74" s="60" customFormat="1" ht="12">
@@ -12874,7 +12831,7 @@
         <v>271</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" s="60" customFormat="1" ht="12"/>
@@ -12929,7 +12886,7 @@
         <v>134</v>
       </c>
       <c r="D4" s="88" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25">
@@ -12940,7 +12897,7 @@
         <v>269</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25">
@@ -12948,7 +12905,7 @@
         <v>246</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -12962,7 +12919,7 @@
         <v>135</v>
       </c>
       <c r="D8" s="88" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -12973,7 +12930,7 @@
         <v>269</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -12981,7 +12938,7 @@
         <v>246</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -12992,10 +12949,10 @@
         <v>268</v>
       </c>
       <c r="C12" s="87" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D12" s="88" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13006,7 +12963,7 @@
         <v>269</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13014,7 +12971,7 @@
         <v>246</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13028,7 +12985,7 @@
         <v>13900000000</v>
       </c>
       <c r="D16" s="88" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13039,7 +12996,7 @@
         <v>269</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13047,7 +13004,7 @@
         <v>246</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13058,10 +13015,10 @@
         <v>268</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D20" s="88" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13072,7 +13029,7 @@
         <v>269</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="74" customFormat="1" ht="14.25">
@@ -13080,7 +13037,7 @@
         <v>246</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -13120,7 +13077,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="104" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25">
@@ -13128,7 +13085,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25">
@@ -13144,7 +13101,7 @@
         <v>246</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -13158,8 +13115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BV15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -13170,12 +13127,12 @@
         <v>86</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:74" s="80" customFormat="1" ht="12">
       <c r="B3" s="83" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C3" s="84" t="s">
         <v>87</v>
@@ -13286,7 +13243,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D5" s="103" t="s">
         <v>180</v>
@@ -13298,25 +13255,25 @@
         <v>192</v>
       </c>
       <c r="G5" s="103" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H5" s="103" t="s">
         <v>259</v>
       </c>
       <c r="I5" s="103" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J5" s="103" t="s">
         <v>259</v>
       </c>
       <c r="K5" s="103" t="s">
+        <v>428</v>
+      </c>
+      <c r="L5" s="103" t="s">
+        <v>429</v>
+      </c>
+      <c r="M5" s="103" t="s">
         <v>430</v>
-      </c>
-      <c r="L5" s="103" t="s">
-        <v>431</v>
-      </c>
-      <c r="M5" s="103" t="s">
-        <v>432</v>
       </c>
       <c r="N5" s="103" t="s">
         <v>169</v>
@@ -13346,7 +13303,7 @@
         <v>77</v>
       </c>
       <c r="W5" s="103" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="X5" s="99" t="s">
         <v>192</v>
@@ -13354,17 +13311,17 @@
       <c r="Y5" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="Z5" s="103" t="s">
-        <v>248</v>
+      <c r="Z5" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA5" s="105" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="AB5" s="103" t="s">
         <v>249</v>
       </c>
       <c r="AC5" s="103" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AD5" s="99" t="s">
         <v>192</v>
@@ -13373,7 +13330,7 @@
         <v>135</v>
       </c>
       <c r="AF5" s="103" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AG5" s="101"/>
       <c r="AH5" s="101"/>
@@ -13421,10 +13378,10 @@
     <row r="6" spans="1:74" s="102" customFormat="1">
       <c r="A6" s="100"/>
       <c r="B6" s="103" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C6" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D6" s="103" t="s">
         <v>180</v>
@@ -13436,13 +13393,13 @@
         <v>90</v>
       </c>
       <c r="G6" s="103" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H6" s="103" t="s">
         <v>260</v>
       </c>
       <c r="I6" s="103" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J6" s="99" t="s">
         <v>192</v>
@@ -13454,7 +13411,7 @@
         <v>90</v>
       </c>
       <c r="M6" s="103" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N6" s="99" t="s">
         <v>192</v>
@@ -13492,8 +13449,8 @@
       <c r="Y6" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="Z6" s="103" t="s">
-        <v>248</v>
+      <c r="Z6" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA6" s="99" t="s">
         <v>90</v>
@@ -13559,10 +13516,10 @@
     <row r="7" spans="1:74" s="102" customFormat="1">
       <c r="A7" s="100"/>
       <c r="B7" s="103" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C7" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D7" s="103" t="s">
         <v>180</v>
@@ -13574,7 +13531,7 @@
         <v>90</v>
       </c>
       <c r="G7" s="103" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H7" s="103" t="s">
         <v>259</v>
@@ -13592,7 +13549,7 @@
         <v>90</v>
       </c>
       <c r="M7" s="103" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N7" s="99" t="s">
         <v>192</v>
@@ -13630,8 +13587,8 @@
       <c r="Y7" s="103" t="s">
         <v>192</v>
       </c>
-      <c r="Z7" s="103" t="s">
-        <v>248</v>
+      <c r="Z7" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA7" s="99" t="s">
         <v>90</v>
@@ -13697,10 +13654,10 @@
     <row r="8" spans="1:74" s="102" customFormat="1">
       <c r="A8" s="100"/>
       <c r="B8" s="103" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D8" s="103" t="s">
         <v>180</v>
@@ -13712,13 +13669,13 @@
         <v>192</v>
       </c>
       <c r="G8" s="103" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H8" s="103" t="s">
         <v>260</v>
       </c>
       <c r="I8" s="103" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J8" s="103" t="s">
         <v>249</v>
@@ -13736,13 +13693,13 @@
         <v>254</v>
       </c>
       <c r="O8" s="103" t="s">
+        <v>399</v>
+      </c>
+      <c r="P8" s="103" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q8" s="103" t="s">
         <v>401</v>
-      </c>
-      <c r="P8" s="103" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q8" s="103" t="s">
-        <v>403</v>
       </c>
       <c r="R8" s="103" t="s">
         <v>207</v>
@@ -13768,8 +13725,8 @@
       <c r="Y8" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="Z8" s="103" t="s">
-        <v>248</v>
+      <c r="Z8" s="112" t="s">
+        <v>573</v>
       </c>
       <c r="AA8" s="99" t="s">
         <v>90</v>
@@ -13778,7 +13735,7 @@
         <v>90</v>
       </c>
       <c r="AC8" s="103" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="AD8" s="99" t="s">
         <v>90</v>
@@ -13787,7 +13744,7 @@
         <v>90</v>
       </c>
       <c r="AF8" s="103" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AG8" s="101"/>
       <c r="AH8" s="101"/>
@@ -13832,13 +13789,15 @@
       <c r="BU8" s="101"/>
       <c r="BV8" s="101"/>
     </row>
-    <row r="9" spans="1:74" s="74" customFormat="1"/>
+    <row r="9" spans="1:74" s="74" customFormat="1">
+      <c r="Z9" s="114"/>
+    </row>
     <row r="10" spans="1:74" s="80" customFormat="1" ht="14.25">
       <c r="A10" s="81" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E10" s="82"/>
       <c r="F10" s="82"/>
@@ -13913,7 +13872,7 @@
     </row>
     <row r="11" spans="1:74" s="80" customFormat="1" ht="12">
       <c r="B11" s="83" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:74" s="80" customFormat="1" ht="12">
@@ -13921,10 +13880,10 @@
         <v>256</v>
       </c>
       <c r="C12" s="77" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:74" s="80" customFormat="1" ht="12">
@@ -13935,7 +13894,7 @@
         <v>271</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:74" s="74" customFormat="1"/>
@@ -13985,13 +13944,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D4" s="88" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="102" customFormat="1" ht="14.25">
@@ -13999,13 +13958,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="102" customFormat="1" ht="14.25">
@@ -14013,13 +13972,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="89" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C6" s="87" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="88" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="102" customFormat="1" ht="14.25">
@@ -14027,13 +13986,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C7" s="87">
         <v>15200000000</v>
       </c>
       <c r="D7" s="88" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25">
@@ -14041,10 +14000,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D8" s="88" t="s">
         <v>317</v>
@@ -14055,13 +14014,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D9" s="88" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25">
@@ -14069,31 +14028,31 @@
         <v>4</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C10" s="87" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D10" s="88" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25">
       <c r="A11" s="85" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C11" s="87"/>
       <c r="D11" s="88"/>
     </row>
     <row r="12" spans="1:4" ht="14.25">
       <c r="A12" s="85" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B12" s="89" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C12" s="87"/>
       <c r="D12" s="88"/>
@@ -14103,13 +14062,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="89" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D13" s="88" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25">
@@ -14117,13 +14076,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="89" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D14" s="88" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25">
@@ -14131,13 +14090,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="89" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C15" s="87">
         <v>11</v>
       </c>
       <c r="D15" s="88" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25">
@@ -14145,13 +14104,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C16" s="87">
         <v>22</v>
       </c>
       <c r="D16" s="88" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25">
@@ -14159,13 +14118,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="89" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C17" s="87">
         <v>33</v>
       </c>
       <c r="D17" s="88" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25">
@@ -14173,13 +14132,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="89" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C18" s="87">
         <v>44</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25">
@@ -14187,29 +14146,29 @@
         <v>4</v>
       </c>
       <c r="B19" s="89" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C19" s="87" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D19" s="88" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25">
       <c r="A21" s="85" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B21" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25">
       <c r="A22" s="85" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B22" s="106" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>